<commit_message>
Anpassungen CDA Release 1.17
</commit_message>
<xml_diff>
--- a/import-server/cda_basismodul/Basismodul-EAV-I2B2.xlsx
+++ b/import-server/cda_basismodul/Basismodul-EAV-I2B2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="291">
   <si>
     <t xml:space="preserve">Feldname </t>
   </si>
@@ -1331,6 +1331,12 @@
   </si>
   <si>
     <t>inhaltliche Abgrenzung 771/808/60; nur 1 davon nehmen; Status zusätzlich?</t>
+  </si>
+  <si>
+    <t>funktioniert nur teilweise, wg. modifier</t>
+  </si>
+  <si>
+    <t>inhaltliche Abgrenzung 771/808/60; nur 1 davon nehmen, Name UND  Nummer?</t>
   </si>
 </sst>
 </file>
@@ -1845,8 +1851,8 @@
   </sheetPr>
   <dimension ref="A1:CC106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="K71" sqref="K71"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="H107" sqref="H107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,7 +2048,7 @@
         <v>275</v>
       </c>
       <c r="J6" s="45" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
@@ -2105,7 +2111,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2251,7 +2257,7 @@
         <v>283</v>
       </c>
       <c r="I13" s="42" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
@@ -2344,7 +2350,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2370,11 +2376,11 @@
         <v>283</v>
       </c>
       <c r="I17" s="35" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="J17" s="44"/>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -2401,10 +2407,10 @@
         <v>283</v>
       </c>
       <c r="I18" s="41" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2436,7 +2442,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -2468,8 +2474,11 @@
       <c r="J20" s="43" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="35" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2496,10 +2505,10 @@
         <v>283</v>
       </c>
       <c r="I21" s="35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>21</v>
       </c>
@@ -2526,10 +2535,10 @@
         <v>283</v>
       </c>
       <c r="I22" s="41" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2556,10 +2565,10 @@
         <v>283</v>
       </c>
       <c r="I23" s="35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>23</v>
       </c>
@@ -2586,10 +2595,10 @@
         <v>283</v>
       </c>
       <c r="I24" s="41" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2616,10 +2625,10 @@
         <v>283</v>
       </c>
       <c r="I25" s="35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>25</v>
       </c>
@@ -2646,10 +2655,10 @@
         <v>283</v>
       </c>
       <c r="I26" s="41" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2676,10 +2685,10 @@
         <v>283</v>
       </c>
       <c r="I27" s="35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>27</v>
       </c>
@@ -2706,10 +2715,10 @@
         <v>283</v>
       </c>
       <c r="I28" s="41" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2736,10 +2745,10 @@
         <v>283</v>
       </c>
       <c r="I29" s="35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>29</v>
       </c>
@@ -2766,10 +2775,10 @@
         <v>283</v>
       </c>
       <c r="I30" s="41" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2796,10 +2805,10 @@
         <v>283</v>
       </c>
       <c r="I31" s="35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>31</v>
       </c>
@@ -2826,7 +2835,7 @@
         <v>283</v>
       </c>
       <c r="I32" s="41" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -2856,10 +2865,10 @@
         <v>283</v>
       </c>
       <c r="I33" s="35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>33</v>
       </c>
@@ -2947,7 +2956,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3211,10 +3220,10 @@
         <v>283</v>
       </c>
       <c r="I45" s="35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>45</v>
       </c>
@@ -3271,7 +3280,7 @@
         <v>283</v>
       </c>
       <c r="I47" s="35" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
     </row>
     <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -3301,7 +3310,7 @@
         <v>283</v>
       </c>
       <c r="I48" s="41" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
     </row>
     <row r="49" spans="1:81" hidden="1" x14ac:dyDescent="0.25">
@@ -3331,10 +3340,10 @@
         <v>283</v>
       </c>
       <c r="I49" s="35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="50" spans="1:81" hidden="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="50" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>49</v>
       </c>
@@ -3456,7 +3465,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:81" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A54" s="12">
         <v>53</v>
       </c>
@@ -3486,7 +3495,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="55" spans="1:81" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -3516,7 +3525,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="56" spans="1:81" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
         <v>55</v>
       </c>
@@ -3545,7 +3554,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="57" spans="1:81" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -3575,7 +3584,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="58" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:81" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12">
         <v>57</v>
       </c>
@@ -3633,7 +3642,7 @@
       </c>
       <c r="J59" s="48"/>
     </row>
-    <row r="60" spans="1:81" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:81" s="13" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
         <v>59</v>
       </c>
@@ -3764,7 +3773,7 @@
         <v>283</v>
       </c>
       <c r="I61" s="45" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="J61" s="45"/>
       <c r="K61" s="45"/>
@@ -4369,7 +4378,7 @@
         <v>283</v>
       </c>
       <c r="I67" s="45" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="J67" s="45"/>
       <c r="K67" s="45"/>
@@ -4471,7 +4480,7 @@
         <v>283</v>
       </c>
       <c r="I68" s="16" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="J68" s="27"/>
       <c r="K68" s="27"/>
@@ -4546,7 +4555,7 @@
       <c r="CB68" s="27"/>
       <c r="CC68" s="27"/>
     </row>
-    <row r="69" spans="1:81" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:81" s="1" customFormat="1" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -4750,7 +4759,7 @@
       <c r="CB70" s="45"/>
       <c r="CC70" s="45"/>
     </row>
-    <row r="71" spans="1:81" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:81" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -4777,7 +4786,7 @@
         <v>283</v>
       </c>
       <c r="I71" s="27" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J71" s="45"/>
       <c r="K71" s="45"/>
@@ -4852,7 +4861,7 @@
       <c r="CB71" s="45"/>
       <c r="CC71" s="45"/>
     </row>
-    <row r="72" spans="1:81" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:81" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12">
         <v>71</v>
       </c>
@@ -5074,7 +5083,7 @@
         <v>283</v>
       </c>
       <c r="I74" s="16" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="J74" s="45"/>
       <c r="K74" s="45"/>
@@ -5149,7 +5158,7 @@
       <c r="CB74" s="45"/>
       <c r="CC74" s="45"/>
     </row>
-    <row r="75" spans="1:81" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:81" s="13" customFormat="1" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -5353,7 +5362,7 @@
       <c r="CB76" s="45"/>
       <c r="CC76" s="45"/>
     </row>
-    <row r="77" spans="1:81" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:81" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -5378,7 +5387,7 @@
         <v>283</v>
       </c>
       <c r="I77" s="27" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J77" s="45"/>
       <c r="K77" s="45"/>
@@ -5453,7 +5462,7 @@
       <c r="CB77" s="45"/>
       <c r="CC77" s="45"/>
     </row>
-    <row r="78" spans="1:81" s="17" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:81" s="17" customFormat="1" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12">
         <v>77</v>
       </c>
@@ -5653,7 +5662,7 @@
       <c r="CB79" s="45"/>
       <c r="CC79" s="45"/>
     </row>
-    <row r="80" spans="1:81" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:81" s="1" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12">
         <v>79</v>
       </c>
@@ -5680,7 +5689,7 @@
         <v>283</v>
       </c>
       <c r="I80" s="16" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J80" s="45"/>
       <c r="K80" s="45"/>
@@ -5755,7 +5764,7 @@
       <c r="CB80" s="45"/>
       <c r="CC80" s="45"/>
     </row>
-    <row r="81" spans="1:81" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:81" s="13" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -5959,7 +5968,7 @@
       <c r="CB82" s="45"/>
       <c r="CC82" s="45"/>
     </row>
-    <row r="83" spans="1:81" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:81" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -5986,7 +5995,7 @@
         <v>283</v>
       </c>
       <c r="I83" s="27" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J83" s="45"/>
       <c r="K83" s="45"/>
@@ -6061,7 +6070,7 @@
       <c r="CB83" s="45"/>
       <c r="CC83" s="45"/>
     </row>
-    <row r="84" spans="1:81" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:81" s="1" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12">
         <v>83</v>
       </c>
@@ -6255,7 +6264,7 @@
       <c r="CB85" s="45"/>
       <c r="CC85" s="45"/>
     </row>
-    <row r="86" spans="1:81" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:81" s="13" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12">
         <v>85</v>
       </c>
@@ -6282,7 +6291,7 @@
         <v>283</v>
       </c>
       <c r="I86" s="16" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J86" s="45"/>
       <c r="K86" s="45"/>
@@ -6357,7 +6366,7 @@
       <c r="CB86" s="45"/>
       <c r="CC86" s="45"/>
     </row>
-    <row r="87" spans="1:81" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:81" s="1" customFormat="1" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -6561,7 +6570,7 @@
       <c r="CB88" s="45"/>
       <c r="CC88" s="45"/>
     </row>
-    <row r="89" spans="1:81" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:81" s="17" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -6588,7 +6597,7 @@
         <v>283</v>
       </c>
       <c r="I89" s="27" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J89" s="45"/>
       <c r="K89" s="45"/>
@@ -6663,7 +6672,7 @@
       <c r="CB89" s="45"/>
       <c r="CC89" s="45"/>
     </row>
-    <row r="90" spans="1:81" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:81" s="13" customFormat="1" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12">
         <v>89</v>
       </c>
@@ -6867,7 +6876,7 @@
       <c r="CB91" s="45"/>
       <c r="CC91" s="45"/>
     </row>
-    <row r="92" spans="1:81" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:81" s="13" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12">
         <v>91</v>
       </c>
@@ -7006,7 +7015,7 @@
       <c r="Q93" s="4"/>
       <c r="R93" s="4"/>
     </row>
-    <row r="94" spans="1:81" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:81" s="13" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12">
         <v>93</v>
       </c>
@@ -7031,7 +7040,7 @@
         <v>283</v>
       </c>
       <c r="I94" s="16" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J94" s="45"/>
       <c r="K94" s="45"/>
@@ -7206,7 +7215,7 @@
       <c r="CB95" s="4"/>
       <c r="CC95" s="4"/>
     </row>
-    <row r="96" spans="1:81" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:81" s="13" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12">
         <v>95</v>
       </c>
@@ -7231,7 +7240,7 @@
         <v>283</v>
       </c>
       <c r="I96" s="16" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J96" s="45"/>
       <c r="K96" s="45"/>
@@ -7406,7 +7415,7 @@
       <c r="CB97" s="45"/>
       <c r="CC97" s="45"/>
     </row>
-    <row r="98" spans="1:81" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:81" s="13" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12">
         <v>97</v>
       </c>
@@ -7431,7 +7440,7 @@
         <v>283</v>
       </c>
       <c r="I98" s="16" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J98" s="45"/>
       <c r="K98" s="45"/>
@@ -7606,7 +7615,7 @@
       <c r="CB99" s="45"/>
       <c r="CC99" s="45"/>
     </row>
-    <row r="100" spans="1:81" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:81" s="13" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12">
         <v>99</v>
       </c>
@@ -7631,7 +7640,7 @@
         <v>283</v>
       </c>
       <c r="I100" s="16" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J100" s="45"/>
       <c r="K100" s="45"/>
@@ -7806,7 +7815,7 @@
       <c r="CB101" s="45"/>
       <c r="CC101" s="45"/>
     </row>
-    <row r="102" spans="1:81" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:81" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12">
         <v>101</v>
       </c>
@@ -7831,7 +7840,7 @@
         <v>283</v>
       </c>
       <c r="I102" s="16" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J102" s="45"/>
       <c r="K102" s="45"/>
@@ -7943,7 +7952,7 @@
       <c r="Q103" s="4"/>
       <c r="R103" s="4"/>
     </row>
-    <row r="104" spans="1:81" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:81" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12">
         <v>103</v>
       </c>
@@ -7968,7 +7977,7 @@
         <v>283</v>
       </c>
       <c r="I104" s="16" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J104" s="45"/>
       <c r="K104" s="45"/>
@@ -8143,7 +8152,7 @@
       <c r="CB105" s="45"/>
       <c r="CC105" s="45"/>
     </row>
-    <row r="106" spans="1:81" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:81" s="13" customFormat="1" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12">
         <v>105</v>
       </c>
@@ -8168,7 +8177,7 @@
         <v>283</v>
       </c>
       <c r="I106" s="16" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="J106" s="45"/>
       <c r="K106" s="45"/>
@@ -8245,12 +8254,11 @@
     </row>
   </sheetData>
   <autoFilter ref="H1:I106">
-    <filterColumn colId="1">
+    <filterColumn colId="0">
       <filters>
-        <filter val="Importieren"/>
+        <filter val="Freitext"/>
         <filter val="ToDo"/>
-        <filter val="Waiting"/>
-        <filter val="Zu klären"/>
+        <filter val="Zu Klären"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>